<commit_message>
updating two stage optimization
</commit_message>
<xml_diff>
--- a/SOO_simulations/DP1000_room_Swift_NDBR50_curve2/iteration/4/parameters.xlsx
+++ b/SOO_simulations/DP1000_room_Swift_NDBR50_curve2/iteration/4/parameters.xlsx
@@ -452,7 +452,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1940.980888274112</v>
+        <v>1306.471719603217</v>
       </c>
     </row>
     <row r="3">
@@ -462,7 +462,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0003225182326382889</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.08922326201700546</v>
+        <v>1.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>